<commit_message>
Committing to new branch.
</commit_message>
<xml_diff>
--- a/OutputFiles/TC06_Canine_Filter_Breed-BelgMalin_Neo4jData.xlsx
+++ b/OutputFiles/TC06_Canine_Filter_Breed-BelgMalin_Neo4jData.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="37">
   <si>
     <t>Case ID</t>
   </si>
@@ -121,6 +121,12 @@
   </si>
   <si>
     <t>MATCH (s:study) WITH COLLECT(DISTINCT(s.clinical_study_designation)) AS all_studies MATCH (d:demographic) WITH COLLECT(DISTINCT(d.breed)) AS all_breeds, COLLECT(DISTINCT(d.sex)) AS all_sexes, all_studies MATCH (d:diagnosis) WITH COLLECT(DISTINCT(d.disease_term)) AS all_diseases, all_breeds, all_sexes, all_studies MATCH (p:program)&lt;-[*]-(s:study)&lt;-[*]-(c:case)&lt;--(demo:demographic), (c)&lt;--(diag:diagnosis) WHERE demo.breed IN['Akita']  OPTIONAL MATCH (f:file)-[*]-&gt;(c), (samp:sample)-[*]-&gt;(c) WITH DISTINCT c AS c, p, s, demo, diag, f, samp RETURN count(DISTINCT(f)) as number_of_files , count(DISTINCT(samp)) as number_of_sample , count(DISTINCT(c.case_id)) as number_of_cases , count(DISTINCT(s.clinical_study_designation)) as number_of_study</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>MATCH (s:study) WITH COLLECT(DISTINCT(s.clinical_study_designation)) AS all_studies MATCH (d:demographic) WITH COLLECT(DISTINCT(d.breed)) AS all_breeds, COLLECT(DISTINCT(d.sex)) AS all_sexes, all_studies MATCH (d:diagnosis) WITH COLLECT(DISTINCT(d.disease_term)) AS all_diseases, all_breeds, all_sexes, all_studies MATCH (p:program)&lt;-[*]-(s:study)&lt;-[*]-(c:case)&lt;--(demo:demographic), (c)&lt;--(diag:diagnosis) WHERE demo.breed IN['Belgian Malinois']  OPTIONAL MATCH (f:file)-[*]-&gt;(c), (samp:sample)-[*]-&gt;(c) WITH DISTINCT c AS c, p, s, demo, diag, f, samp RETURN count(DISTINCT(f)) as number_of_files , count(DISTINCT(samp)) as number_of_sample , count(DISTINCT(c.case_id)) as number_of_cases , count(DISTINCT(s.clinical_study_designation)) as number_of_study</t>
   </si>
 </sst>
 </file>
@@ -384,10 +390,10 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="B2" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C2" t="s">
         <v>32</v>
@@ -496,7 +502,7 @@
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="19">

</xml_diff>